<commit_message>
fixed : #1 로직 수정중
</commit_message>
<xml_diff>
--- a/DragAndDrop/Assets/06.Data/Excel/Stage2/Stage2_Shot_excel.xlsx
+++ b/DragAndDrop/Assets/06.Data/Excel/Stage2/Stage2_Shot_excel.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.junheeStudy\Team_Project\idle\DragAndDrop\Assets\06.Data\Excel\Stage2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shingu104\Desktop\idle\DragAndDrop\Assets\06.Data\Excel\Stage2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737D85F0-B0AA-471D-9163-C2AF3BA59D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63912014-BF4A-4F18-852E-8D74DAEBE5CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,11 +429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2C8B6B-81C9-4B21-8DB2-E0724AABC855}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1060,7 +1059,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>45.65</v>
+        <v>44.7</v>
       </c>
       <c r="B57" s="1">
         <v>6</v>

</xml_diff>